<commit_message>
chAnge integration container to prepare
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Bond.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Bond.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7202E4E-0D50-7F40-9D34-7A8EC7BB841A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758CF6B6-BB97-CF41-9CB5-1CD39EC486E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,11 +313,10 @@
     <t>uid</t>
   </si>
   <si>
-    <t>business_rules</t>
+    <t>sync</t>
   </si>
   <si>
-    <t>reindex_lookup_bond_providers
-convert_to_int</t>
+    <t>sync_lookup</t>
   </si>
 </sst>
 </file>
@@ -711,7 +710,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1066,7 +1065,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
add the rest of the table defs
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Bond.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Bond.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBD0A36-BEA8-6246-AC43-ED0E4F348649}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D11A9-A9A5-CD4C-BEC2-0038E45808CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="bonds" sheetId="1" r:id="rId1"/>
-    <sheet name="bond_status_lookup" sheetId="2" r:id="rId2"/>
-    <sheet name="bond_provider_lookup" sheetId="3" r:id="rId3"/>
-    <sheet name="bond_required_lookup" sheetId="4" r:id="rId4"/>
-    <sheet name="bond_providers" sheetId="5" r:id="rId5"/>
+    <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
+    <sheet name="bonds" sheetId="1" r:id="rId2"/>
+    <sheet name="bond_status_lookup" sheetId="2" r:id="rId3"/>
+    <sheet name="bond_provider_lookup" sheetId="3" r:id="rId4"/>
+    <sheet name="bond_required_lookup" sheetId="4" r:id="rId5"/>
+    <sheet name="bond_providers" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
   <si>
     <t>table_name</t>
   </si>
@@ -331,6 +332,42 @@
   <si>
     <t>sync_lookup</t>
   </si>
+  <si>
+    <t>mapping_file_name</t>
+  </si>
+  <si>
+    <t>entity_name</t>
+  </si>
+  <si>
+    <t>required_entities</t>
+  </si>
+  <si>
+    <t>destination_table_name</t>
+  </si>
+  <si>
+    <t>table_type</t>
+  </si>
+  <si>
+    <t>source_table_name</t>
+  </si>
+  <si>
+    <t>casrec_conditions</t>
+  </si>
+  <si>
+    <t>source_table_additional_columns</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Bond No. = not null</t>
+  </si>
+  <si>
+    <t>CoP Case</t>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +376,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -387,6 +424,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -462,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -492,6 +535,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +751,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13601406-4B41-724C-BED5-8579D7BE162F}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
     </sheetView>
@@ -2534,7 +2644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -9068,7 +9178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -9373,1568 +9483,6 @@
       <c r="D24" s="14">
         <v>43757</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="8"/>
-    </row>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="8"/>
-    </row>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="8"/>
-    </row>
-    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="8"/>
-    </row>
-    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="8"/>
-    </row>
-    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="8"/>
-    </row>
-    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="8"/>
-    </row>
-    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="8"/>
-    </row>
-    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="8"/>
-    </row>
-    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="8"/>
-    </row>
-    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="8"/>
-    </row>
-    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="8"/>
-    </row>
-    <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B55" s="8"/>
-    </row>
-    <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="8"/>
-    </row>
-    <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="8"/>
-    </row>
-    <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="8"/>
-    </row>
-    <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B60" s="8"/>
-    </row>
-    <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B61" s="8"/>
-    </row>
-    <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B62" s="8"/>
-    </row>
-    <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B63" s="8"/>
-    </row>
-    <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B64" s="8"/>
-    </row>
-    <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B65" s="8"/>
-    </row>
-    <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B66" s="8"/>
-    </row>
-    <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B67" s="8"/>
-    </row>
-    <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B68" s="8"/>
-    </row>
-    <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B69" s="8"/>
-    </row>
-    <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B70" s="8"/>
-    </row>
-    <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B71" s="8"/>
-    </row>
-    <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B72" s="8"/>
-    </row>
-    <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B73" s="8"/>
-    </row>
-    <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B74" s="8"/>
-    </row>
-    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B75" s="8"/>
-    </row>
-    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B76" s="8"/>
-    </row>
-    <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B77" s="8"/>
-    </row>
-    <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B78" s="8"/>
-    </row>
-    <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B79" s="8"/>
-    </row>
-    <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B80" s="8"/>
-    </row>
-    <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B81" s="8"/>
-    </row>
-    <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B82" s="8"/>
-    </row>
-    <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B83" s="8"/>
-    </row>
-    <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B84" s="8"/>
-    </row>
-    <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B85" s="8"/>
-    </row>
-    <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B86" s="8"/>
-    </row>
-    <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B87" s="8"/>
-    </row>
-    <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B88" s="8"/>
-    </row>
-    <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B89" s="8"/>
-    </row>
-    <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B90" s="8"/>
-    </row>
-    <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B91" s="8"/>
-    </row>
-    <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B92" s="8"/>
-    </row>
-    <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B93" s="8"/>
-    </row>
-    <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B94" s="8"/>
-    </row>
-    <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B95" s="8"/>
-    </row>
-    <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B96" s="8"/>
-    </row>
-    <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B97" s="8"/>
-    </row>
-    <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B98" s="8"/>
-    </row>
-    <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B99" s="8"/>
-    </row>
-    <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B100" s="8"/>
-    </row>
-    <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B101" s="8"/>
-    </row>
-    <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B102" s="8"/>
-    </row>
-    <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B103" s="8"/>
-    </row>
-    <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B104" s="8"/>
-    </row>
-    <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B105" s="8"/>
-    </row>
-    <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B106" s="8"/>
-    </row>
-    <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B107" s="8"/>
-    </row>
-    <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B108" s="8"/>
-    </row>
-    <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B109" s="8"/>
-    </row>
-    <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B110" s="8"/>
-    </row>
-    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B111" s="8"/>
-    </row>
-    <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B112" s="8"/>
-    </row>
-    <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B113" s="8"/>
-    </row>
-    <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B114" s="8"/>
-    </row>
-    <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B115" s="8"/>
-    </row>
-    <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B116" s="8"/>
-    </row>
-    <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B117" s="8"/>
-    </row>
-    <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B118" s="8"/>
-    </row>
-    <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B119" s="8"/>
-    </row>
-    <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B120" s="8"/>
-    </row>
-    <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B121" s="8"/>
-    </row>
-    <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B122" s="8"/>
-    </row>
-    <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B123" s="8"/>
-    </row>
-    <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B124" s="8"/>
-    </row>
-    <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B125" s="8"/>
-    </row>
-    <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B126" s="8"/>
-    </row>
-    <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B127" s="8"/>
-    </row>
-    <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B128" s="8"/>
-    </row>
-    <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B129" s="8"/>
-    </row>
-    <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B130" s="8"/>
-    </row>
-    <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B131" s="8"/>
-    </row>
-    <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B132" s="8"/>
-    </row>
-    <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B133" s="8"/>
-    </row>
-    <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B134" s="8"/>
-    </row>
-    <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B135" s="8"/>
-    </row>
-    <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B136" s="8"/>
-    </row>
-    <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B137" s="8"/>
-    </row>
-    <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B138" s="8"/>
-    </row>
-    <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B139" s="8"/>
-    </row>
-    <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B140" s="8"/>
-    </row>
-    <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B141" s="8"/>
-    </row>
-    <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B142" s="8"/>
-    </row>
-    <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B143" s="8"/>
-    </row>
-    <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B144" s="8"/>
-    </row>
-    <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B145" s="8"/>
-    </row>
-    <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B146" s="8"/>
-    </row>
-    <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B147" s="8"/>
-    </row>
-    <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B148" s="8"/>
-    </row>
-    <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B149" s="8"/>
-    </row>
-    <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B150" s="8"/>
-    </row>
-    <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B151" s="8"/>
-    </row>
-    <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B152" s="8"/>
-    </row>
-    <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B153" s="8"/>
-    </row>
-    <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B154" s="8"/>
-    </row>
-    <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B155" s="8"/>
-    </row>
-    <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B156" s="8"/>
-    </row>
-    <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B157" s="8"/>
-    </row>
-    <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B158" s="8"/>
-    </row>
-    <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B159" s="8"/>
-    </row>
-    <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B160" s="8"/>
-    </row>
-    <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B161" s="8"/>
-    </row>
-    <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B162" s="8"/>
-    </row>
-    <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B163" s="8"/>
-    </row>
-    <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B164" s="8"/>
-    </row>
-    <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B165" s="8"/>
-    </row>
-    <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B166" s="8"/>
-    </row>
-    <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B167" s="8"/>
-    </row>
-    <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B168" s="8"/>
-    </row>
-    <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B169" s="8"/>
-    </row>
-    <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B170" s="8"/>
-    </row>
-    <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B171" s="8"/>
-    </row>
-    <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B172" s="8"/>
-    </row>
-    <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B173" s="8"/>
-    </row>
-    <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B174" s="8"/>
-    </row>
-    <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B175" s="8"/>
-    </row>
-    <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B176" s="8"/>
-    </row>
-    <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B177" s="8"/>
-    </row>
-    <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B178" s="8"/>
-    </row>
-    <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B179" s="8"/>
-    </row>
-    <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B180" s="8"/>
-    </row>
-    <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B181" s="8"/>
-    </row>
-    <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B182" s="8"/>
-    </row>
-    <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B183" s="8"/>
-    </row>
-    <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B184" s="8"/>
-    </row>
-    <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B185" s="8"/>
-    </row>
-    <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B186" s="8"/>
-    </row>
-    <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B187" s="8"/>
-    </row>
-    <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B188" s="8"/>
-    </row>
-    <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B189" s="8"/>
-    </row>
-    <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B190" s="8"/>
-    </row>
-    <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B191" s="8"/>
-    </row>
-    <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B192" s="8"/>
-    </row>
-    <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B193" s="8"/>
-    </row>
-    <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B194" s="8"/>
-    </row>
-    <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B195" s="8"/>
-    </row>
-    <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B196" s="8"/>
-    </row>
-    <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B197" s="8"/>
-    </row>
-    <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B198" s="8"/>
-    </row>
-    <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B199" s="8"/>
-    </row>
-    <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B200" s="8"/>
-    </row>
-    <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B201" s="8"/>
-    </row>
-    <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B202" s="8"/>
-    </row>
-    <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B203" s="8"/>
-    </row>
-    <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B204" s="8"/>
-    </row>
-    <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B205" s="8"/>
-    </row>
-    <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B206" s="8"/>
-    </row>
-    <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B207" s="8"/>
-    </row>
-    <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B208" s="8"/>
-    </row>
-    <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B209" s="8"/>
-    </row>
-    <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B210" s="8"/>
-    </row>
-    <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B211" s="8"/>
-    </row>
-    <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B212" s="8"/>
-    </row>
-    <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B213" s="8"/>
-    </row>
-    <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B214" s="8"/>
-    </row>
-    <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B215" s="8"/>
-    </row>
-    <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B216" s="8"/>
-    </row>
-    <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B217" s="8"/>
-    </row>
-    <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B218" s="8"/>
-    </row>
-    <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B219" s="8"/>
-    </row>
-    <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B220" s="8"/>
-    </row>
-    <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B221" s="8"/>
-    </row>
-    <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B222" s="8"/>
-    </row>
-    <row r="223" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B223" s="8"/>
-    </row>
-    <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B224" s="8"/>
-    </row>
-    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" customWidth="1"/>
-    <col min="4" max="6" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="8"/>
@@ -12319,6 +10867,1568 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:D1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" customWidth="1"/>
+    <col min="4" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="8"/>
+    </row>
+    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="8"/>
+    </row>
+    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="8"/>
+    </row>
+    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="8"/>
+    </row>
+    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="8"/>
+    </row>
+    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="8"/>
+    </row>
+    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" s="8"/>
+    </row>
+    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="8"/>
+    </row>
+    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="8"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B53" s="8"/>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="8"/>
+    </row>
+    <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="8"/>
+    </row>
+    <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="8"/>
+    </row>
+    <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B57" s="8"/>
+    </row>
+    <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="8"/>
+    </row>
+    <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="8"/>
+    </row>
+    <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B60" s="8"/>
+    </row>
+    <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B61" s="8"/>
+    </row>
+    <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B62" s="8"/>
+    </row>
+    <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B63" s="8"/>
+    </row>
+    <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" s="8"/>
+    </row>
+    <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B68" s="8"/>
+    </row>
+    <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B69" s="8"/>
+    </row>
+    <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B70" s="8"/>
+    </row>
+    <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B71" s="8"/>
+    </row>
+    <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B72" s="8"/>
+    </row>
+    <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73" s="8"/>
+    </row>
+    <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B75" s="8"/>
+    </row>
+    <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="8"/>
+    </row>
+    <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B77" s="8"/>
+    </row>
+    <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B78" s="8"/>
+    </row>
+    <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B79" s="8"/>
+    </row>
+    <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B80" s="8"/>
+    </row>
+    <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B81" s="8"/>
+    </row>
+    <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="8"/>
+    </row>
+    <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B83" s="8"/>
+    </row>
+    <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B84" s="8"/>
+    </row>
+    <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B85" s="8"/>
+    </row>
+    <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B86" s="8"/>
+    </row>
+    <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B87" s="8"/>
+    </row>
+    <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B88" s="8"/>
+    </row>
+    <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B89" s="8"/>
+    </row>
+    <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B90" s="8"/>
+    </row>
+    <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B91" s="8"/>
+    </row>
+    <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B92" s="8"/>
+    </row>
+    <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B93" s="8"/>
+    </row>
+    <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B94" s="8"/>
+    </row>
+    <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B95" s="8"/>
+    </row>
+    <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B96" s="8"/>
+    </row>
+    <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B97" s="8"/>
+    </row>
+    <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B98" s="8"/>
+    </row>
+    <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B99" s="8"/>
+    </row>
+    <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B100" s="8"/>
+    </row>
+    <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B101" s="8"/>
+    </row>
+    <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B102" s="8"/>
+    </row>
+    <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B103" s="8"/>
+    </row>
+    <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B104" s="8"/>
+    </row>
+    <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B105" s="8"/>
+    </row>
+    <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B106" s="8"/>
+    </row>
+    <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B107" s="8"/>
+    </row>
+    <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B108" s="8"/>
+    </row>
+    <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B109" s="8"/>
+    </row>
+    <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B110" s="8"/>
+    </row>
+    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B111" s="8"/>
+    </row>
+    <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B112" s="8"/>
+    </row>
+    <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B113" s="8"/>
+    </row>
+    <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B114" s="8"/>
+    </row>
+    <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B115" s="8"/>
+    </row>
+    <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B116" s="8"/>
+    </row>
+    <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B117" s="8"/>
+    </row>
+    <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B118" s="8"/>
+    </row>
+    <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B119" s="8"/>
+    </row>
+    <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B120" s="8"/>
+    </row>
+    <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B121" s="8"/>
+    </row>
+    <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B122" s="8"/>
+    </row>
+    <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B123" s="8"/>
+    </row>
+    <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B124" s="8"/>
+    </row>
+    <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B125" s="8"/>
+    </row>
+    <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B126" s="8"/>
+    </row>
+    <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B127" s="8"/>
+    </row>
+    <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B128" s="8"/>
+    </row>
+    <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B129" s="8"/>
+    </row>
+    <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B130" s="8"/>
+    </row>
+    <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B131" s="8"/>
+    </row>
+    <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B132" s="8"/>
+    </row>
+    <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B133" s="8"/>
+    </row>
+    <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B134" s="8"/>
+    </row>
+    <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B135" s="8"/>
+    </row>
+    <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B136" s="8"/>
+    </row>
+    <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B137" s="8"/>
+    </row>
+    <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B138" s="8"/>
+    </row>
+    <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B139" s="8"/>
+    </row>
+    <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B140" s="8"/>
+    </row>
+    <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B141" s="8"/>
+    </row>
+    <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B142" s="8"/>
+    </row>
+    <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B143" s="8"/>
+    </row>
+    <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B144" s="8"/>
+    </row>
+    <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B145" s="8"/>
+    </row>
+    <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B146" s="8"/>
+    </row>
+    <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B147" s="8"/>
+    </row>
+    <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B148" s="8"/>
+    </row>
+    <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B149" s="8"/>
+    </row>
+    <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B150" s="8"/>
+    </row>
+    <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B151" s="8"/>
+    </row>
+    <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B152" s="8"/>
+    </row>
+    <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B153" s="8"/>
+    </row>
+    <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B154" s="8"/>
+    </row>
+    <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B155" s="8"/>
+    </row>
+    <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B156" s="8"/>
+    </row>
+    <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B157" s="8"/>
+    </row>
+    <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B158" s="8"/>
+    </row>
+    <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B159" s="8"/>
+    </row>
+    <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B160" s="8"/>
+    </row>
+    <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B161" s="8"/>
+    </row>
+    <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B162" s="8"/>
+    </row>
+    <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B163" s="8"/>
+    </row>
+    <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B164" s="8"/>
+    </row>
+    <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B165" s="8"/>
+    </row>
+    <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B166" s="8"/>
+    </row>
+    <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B167" s="8"/>
+    </row>
+    <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B168" s="8"/>
+    </row>
+    <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B169" s="8"/>
+    </row>
+    <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B170" s="8"/>
+    </row>
+    <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B171" s="8"/>
+    </row>
+    <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B172" s="8"/>
+    </row>
+    <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B173" s="8"/>
+    </row>
+    <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B174" s="8"/>
+    </row>
+    <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B175" s="8"/>
+    </row>
+    <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B176" s="8"/>
+    </row>
+    <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B177" s="8"/>
+    </row>
+    <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B178" s="8"/>
+    </row>
+    <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B179" s="8"/>
+    </row>
+    <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B180" s="8"/>
+    </row>
+    <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B181" s="8"/>
+    </row>
+    <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B182" s="8"/>
+    </row>
+    <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B183" s="8"/>
+    </row>
+    <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B184" s="8"/>
+    </row>
+    <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B185" s="8"/>
+    </row>
+    <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B186" s="8"/>
+    </row>
+    <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B187" s="8"/>
+    </row>
+    <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B188" s="8"/>
+    </row>
+    <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B189" s="8"/>
+    </row>
+    <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B190" s="8"/>
+    </row>
+    <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B191" s="8"/>
+    </row>
+    <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B192" s="8"/>
+    </row>
+    <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B193" s="8"/>
+    </row>
+    <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B194" s="8"/>
+    </row>
+    <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B195" s="8"/>
+    </row>
+    <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B196" s="8"/>
+    </row>
+    <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B197" s="8"/>
+    </row>
+    <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B198" s="8"/>
+    </row>
+    <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B199" s="8"/>
+    </row>
+    <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B200" s="8"/>
+    </row>
+    <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B201" s="8"/>
+    </row>
+    <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B202" s="8"/>
+    </row>
+    <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B203" s="8"/>
+    </row>
+    <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B204" s="8"/>
+    </row>
+    <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B205" s="8"/>
+    </row>
+    <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B206" s="8"/>
+    </row>
+    <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B207" s="8"/>
+    </row>
+    <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B208" s="8"/>
+    </row>
+    <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B209" s="8"/>
+    </row>
+    <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B210" s="8"/>
+    </row>
+    <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B211" s="8"/>
+    </row>
+    <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B212" s="8"/>
+    </row>
+    <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B213" s="8"/>
+    </row>
+    <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B214" s="8"/>
+    </row>
+    <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B215" s="8"/>
+    </row>
+    <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B216" s="8"/>
+    </row>
+    <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B217" s="8"/>
+    </row>
+    <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B218" s="8"/>
+    </row>
+    <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B219" s="8"/>
+    </row>
+    <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B220" s="8"/>
+    </row>
+    <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B221" s="8"/>
+    </row>
+    <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B222" s="8"/>
+    </row>
+    <row r="223" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B223" s="8"/>
+    </row>
+    <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B224" s="8"/>
+    </row>
+    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
bonds source conditions tweak
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Bond.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Bond.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D11A9-A9A5-CD4C-BEC2-0038E45808CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED71D63C-F168-A248-B1CE-95A3457A7C88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,10 +363,10 @@
     <t>order</t>
   </si>
   <si>
-    <t>Bond No. = not null</t>
+    <t>Bond Rqd = Y</t>
   </si>
   <si>
-    <t>CoP Case</t>
+    <t>CoP Case, Bond Rqd</t>
   </si>
 </sst>
 </file>
@@ -755,7 +755,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>